<commit_message>
add new test script
</commit_message>
<xml_diff>
--- a/testcases/homepage_result.xlsx
+++ b/testcases/homepage_result.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
-    <t>rsp_code</t>
+    <t>返回</t>
   </si>
   <si>
     <t>0000</t>
@@ -25,19 +25,19 @@
     <t>timestamp</t>
   </si>
   <si>
-    <t>20160608174832541</t>
+    <t>20160613142252837</t>
   </si>
   <si>
     <t>sign</t>
   </si>
   <si>
-    <t>4a510f2bcd1ca09ccf377c91a50177b9</t>
+    <t>8e41c798b25d0a14e35374aa453e1bb9</t>
   </si>
   <si>
     <t>buyback_scan</t>
   </si>
   <si>
-    <t>/advertisement/20160518/2016051817202293522.jpg</t>
+    <t>/advertisement/20160612/2016061215050126629.png</t>
   </si>
   <si>
     <t>rsp_msg</t>

</xml_diff>